<commit_message>
Repository Interface 추가 및 개선 수정중
</commit_message>
<xml_diff>
--- a/Document/04.V1.0_Ciagoar_REQ_DOC.xlsx
+++ b/Document/04.V1.0_Ciagoar_REQ_DOC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\005.Source\Ciagoar\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FA7CF8B-0923-4DB9-AAD0-4CB64567E201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B292D37-3E4D-4484-BBF0-4B3153634260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA8E41B0-9E14-4431-B8E9-CD3124796D11}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA8E41B0-9E14-4431-B8E9-CD3124796D11}"/>
   </bookViews>
   <sheets>
     <sheet name="CIAGOAR" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="119">
   <si>
     <t>요구사항 ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,30 +191,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>REQ004_RCOSEARCH01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ004_RCOSEARCH02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ004_RCOMODI01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ004_RCODROP01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>REQ003_UDROP01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>REQ004_RCOSEARCH03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>관계사들 리스트가 조회가능해야한다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -251,11 +231,272 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>개발진척</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
+    <t>REQ010</t>
+  </si>
+  <si>
+    <t>REQ011</t>
+  </si>
+  <si>
+    <t>REQ012</t>
+  </si>
+  <si>
+    <t>REQ013</t>
+  </si>
+  <si>
+    <t>물품등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품 등록 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품정보,제조사ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장소등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장소수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장소삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고정보등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고정보수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고정보삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ014</t>
+  </si>
+  <si>
+    <t>REQ015</t>
+  </si>
+  <si>
+    <t>물품 수정 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품 삭제 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장소 등록 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장소 수정 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장소 삭제 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고 수정 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고 삭제 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관계사와 연관된 물품 정보가 등록 가능해야한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">등록된 물품의 수정이 가능해야 한다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 물품의 삭제가 가능해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ016</t>
+  </si>
+  <si>
+    <t>물품조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ005_RCOSRC01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ005_RCOSRC02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ005_RCOSRC03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품 조회 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 물품 정보들의 조회가 가능해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ017</t>
+  </si>
+  <si>
+    <t>저장소조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장소 조회 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 저장소 정보들의 조회가 가능해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관계사와 연관된 저장소 정보가 등록 가능해야한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">등록된 저장소의 수정이 가능해야 한다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 저장소의 삭제가 가능해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고정보조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ018</t>
+  </si>
+  <si>
+    <t>REQ019</t>
+  </si>
+  <si>
+    <t>REQ020</t>
+  </si>
+  <si>
+    <t>REQ007_RCOMODI01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ008_RCODROP01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ009_ITEMSRC01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ010_ITEMADD01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ011_ITEMMOD01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ012_ITEMDEL01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ013_STORAGESRC01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ014_STORAGEADD01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ015_STORAGEMOD01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ016_STORAGEDEL01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ017_INVENSRC01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ018_INVENADD01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ019_INVENMOD01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ020_INVENDEL01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고 조회 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고 등록 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 재고 정보들의 조회가 가능해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관계사와 연관된 재고 정보가 등록 가능해야한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">등록된 재고의 수정이 가능해야 한다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 재고의 삭제가 가능해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장소 정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품정보,저장소정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -323,7 +564,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -346,12 +587,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -671,24 +909,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89564F3F-7103-4ED3-876B-0AC70135467E}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -710,251 +948,464 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7" t="s">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>49</v>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="9" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="10" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="10" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="10" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="10" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="C15" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>